<commit_message>
Sheet names are updated.
</commit_message>
<xml_diff>
--- a/automotive/automotive-consumer-feedbacks-turkish.xlsx
+++ b/automotive/automotive-consumer-feedbacks-turkish.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ML-Model-Github_DataSet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafa/Projects/kimola-cognitive-datasets/automotive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91610642-8DC8-40A3-8CA8-5BF6B00E872A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1315A276-6DF5-3643-AD60-3B1D8843DDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9A299844-98EA-4873-B169-A2554960A6F8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{9A299844-98EA-4873-B169-A2554960A6F8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
+    <sheet name="Conversations" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -725,512 +725,512 @@
       <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="149.109375" customWidth="1"/>
+    <col min="1" max="1" width="149.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>100</v>
       </c>

</xml_diff>